<commit_message>
added test data for CAN
</commit_message>
<xml_diff>
--- a/Bootstrap/VT-ACH-Data.xlsx
+++ b/Bootstrap/VT-ACH-Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\Bootstrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1266FC79-F9B1-423F-9468-392A4F8A41FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FFA061-B164-4DF0-854A-48B78341EAD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="884" firstSheet="12" activeTab="15" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="884" xr2:uid="{3836B69F-85F5-4D65-8F1B-FC37FA075D01}"/>
   </bookViews>
   <sheets>
     <sheet name="VT-ACHPersonal-NoCF-Generic" sheetId="1" r:id="rId1"/>
@@ -787,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C179FDD-E618-4742-8F86-80396375312B}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
       <selection activeCell="Q1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -3603,7 +3603,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0973E4DA-EDA8-4F1C-A4F8-23673FA64EB4}">
   <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>

</xml_diff>